<commit_message>
Them mot so tap tin moi
</commit_message>
<xml_diff>
--- a/ThongTin.xlsx
+++ b/ThongTin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell Pro\Desktop\DoAnKTLT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell Pro\Desktop\DoAnKTLT\Do-An-KTLT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96284669-FC93-48E2-983A-AF3CF32D909F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFEFCCC-A34F-421D-9B14-EDCC21598D32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>13/04/1999</t>
   </si>
@@ -170,13 +170,43 @@
   </si>
   <si>
     <t>Nghe nhạc và chơi game</t>
+  </si>
+  <si>
+    <t>vy@gmail.com</t>
+  </si>
+  <si>
+    <t>dvinh@gmail.com</t>
+  </si>
+  <si>
+    <t>vuong@gmail.com</t>
+  </si>
+  <si>
+    <t>nvinh@gmail.com</t>
+  </si>
+  <si>
+    <t>vi@gmail.com</t>
+  </si>
+  <si>
+    <t>tvy@gmail.com</t>
+  </si>
+  <si>
+    <t>viet@gmail.com</t>
+  </si>
+  <si>
+    <t>tvi@gmail.com</t>
+  </si>
+  <si>
+    <t>tvu@gmail.com</t>
+  </si>
+  <si>
+    <t>hvu@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +337,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -609,7 +647,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -652,13 +690,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -692,6 +732,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1012,7 +1053,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1020,291 +1061,333 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="2" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1712928</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>2017</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1712908</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2017</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1712925</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2017</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1712914</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2017</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1712902</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>2017</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1712929</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2017</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1712923</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>2017</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1712907</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2017</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1712900</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2017</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>42</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1712924</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2017</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>47</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{ECA4BCB3-FEAA-4B0E-A5E2-8D55BAF69DBB}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{7D6F287C-772E-48D3-9405-68CEEFD6CC8E}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{95090B1E-75ED-4939-B2D6-FE5A38FE98A3}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{30C2BB6F-AC42-42D1-A400-A4CC2489E9EC}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{13143341-663D-472D-8E99-64C87637B831}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{36CA808D-BDB3-456F-80D0-31A65C7F11C6}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{BA5CA536-6217-4A9C-8D5E-2CCDB94AA3C3}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{0948EFCC-28BC-4F94-A358-8C3F0EE4DD73}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{8162F234-CE11-4640-8D72-8C45899297EC}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{F3FA5B3A-3BC3-4EF2-97E3-69A3A888BF86}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>